<commit_message>
Corrige errores en el archivo de datos
</commit_message>
<xml_diff>
--- a/tests/data/datos_pruebas/IG_POSICION_TRAMPAS_14JUN2020.xlsx
+++ b/tests/data/datos_pruebas/IG_POSICION_TRAMPAS_14JUN2020.xlsx
@@ -29,12 +29,12 @@
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Coor-A</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coor-X</t>
   </si>
   <si>
+    <t xml:space="preserve">Coor-Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nombre del responsable</t>
   </si>
   <si>
@@ -2018,13 +2018,13 @@
     <t xml:space="preserve">TC-03-010-TA</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-03-014-LlE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-03-016-LlE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-03-017-LlE</t>
+    <t xml:space="preserve">TC-03-014-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-03-016-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-03-017-LE</t>
   </si>
   <si>
     <t xml:space="preserve">TC-03-018-JC</t>
@@ -3050,19 +3050,19 @@
     <t xml:space="preserve">TC-05-021-LE</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-05-022-LlE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-05-023-LlE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-05-024-LlE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-05-025-LlE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-05-026-LlE</t>
+    <t xml:space="preserve">TC-05-022-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-05-023-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-05-024-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-05-025-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-05-026-LE</t>
   </si>
   <si>
     <t xml:space="preserve">TC-05-027-JR</t>
@@ -3920,10 +3920,10 @@
     <t xml:space="preserve">TC-07-015-DG</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-07-015-LlE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC-07-016-LlE</t>
+    <t xml:space="preserve">TC-07-015-LE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC-07-016-LE</t>
   </si>
   <si>
     <t xml:space="preserve">TC-07-016-PC</t>
@@ -3932,13 +3932,13 @@
     <t xml:space="preserve">TC-07-018-DG</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-07-018-LlE</t>
+    <t xml:space="preserve">TC-07-018-LE</t>
   </si>
   <si>
     <t xml:space="preserve">TC-07-019-DG</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-07-019-LlE</t>
+    <t xml:space="preserve">TC-07-019-LE</t>
   </si>
   <si>
     <t xml:space="preserve">TC-07-020-CRA</t>
@@ -4922,7 +4922,7 @@
     <t xml:space="preserve">TT-02-001-MV</t>
   </si>
   <si>
-    <t xml:space="preserve">TT-03-015-LlE</t>
+    <t xml:space="preserve">TT-03-015-LE</t>
   </si>
   <si>
     <t xml:space="preserve">TT-04-043-MD</t>
@@ -5009,7 +5009,7 @@
     <t xml:space="preserve">TT-07-006-CF</t>
   </si>
   <si>
-    <t xml:space="preserve">TT-07-017-LlE</t>
+    <t xml:space="preserve">TT-07-017-LE</t>
   </si>
 </sst>
 </file>
@@ -5569,12 +5569,12 @@
   <dimension ref="A1:K1640"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L56" activeCellId="0" sqref="L56"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="7" sqref="A643:A645 A987:A991 A1277:A1278 A1281 A1283 A1611 A1640 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.43"/>
@@ -5585,7 +5585,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1017" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -63088,10 +63088,10 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="7" sqref="A643:A645 A987:A991 A1277:A1278 A1281 A1283 A1611 A1640 C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">

</xml_diff>

<commit_message>
Corrige errores en archivo de datos
</commit_message>
<xml_diff>
--- a/tests/data/datos_pruebas/IG_POSICION_TRAMPAS_14JUN2020.xlsx
+++ b/tests/data/datos_pruebas/IG_POSICION_TRAMPAS_14JUN2020.xlsx
@@ -2846,7 +2846,7 @@
     <t xml:space="preserve">TC-04-180-CE</t>
   </si>
   <si>
-    <t xml:space="preserve">TC-04-181-k9</t>
+    <t xml:space="preserve">TC-04-181-K9</t>
   </si>
   <si>
     <t xml:space="preserve">TC-04-182-JCR</t>
@@ -4916,7 +4916,7 @@
     <t xml:space="preserve">TL-08-020-DG</t>
   </si>
   <si>
-    <t xml:space="preserve">TT-01-01-AG</t>
+    <t xml:space="preserve">TT-01-001-AG</t>
   </si>
   <si>
     <t xml:space="preserve">TT-02-001-MV</t>
@@ -5571,10 +5571,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="7" sqref="A643:A645 A987:A991 A1277:A1278 A1281 A1283 A1611 A1640 A1"/>
+      <selection pane="bottomLeft" activeCell="A1641" activeCellId="0" sqref="A1641"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.43"/>
@@ -63088,10 +63088,10 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="7" sqref="A643:A645 A987:A991 A1277:A1278 A1281 A1283 A1611 A1640 C19"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="13" t="s">

</xml_diff>